<commit_message>
Mise à jour complete - donnees jusqu au 2 fevrier 2026
</commit_message>
<xml_diff>
--- a/reports/ReportHistory-10960352.xlsx
+++ b/reports/ReportHistory-10960352.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N194"/>
+  <dimension ref="A1:N214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026.01.26 06:10</t>
+          <t>2026.02.03 06:10</t>
         </is>
       </c>
     </row>
@@ -9528,6 +9528,966 @@
       <c r="N194" t="inlineStr">
         <is>
           <t>[tp 864.01]</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2026.01.26 10:35:52</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>705535092</v>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F195" t="n">
+        <v>0.69163</v>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>2026.01.26 18:16:55</t>
+        </is>
+      </c>
+      <c r="J195" t="n">
+        <v>0.6933</v>
+      </c>
+      <c r="K195" t="n">
+        <v>0</v>
+      </c>
+      <c r="L195" t="n">
+        <v>0</v>
+      </c>
+      <c r="M195" t="n">
+        <v>156.98</v>
+      </c>
+      <c r="N195" t="inlineStr">
+        <is>
+          <t>[sl 0.69330]</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2026.01.26 11:05:42</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>705627973</v>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F196" t="n">
+        <v>0.69154</v>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>2026.01.26 18:16:55</t>
+        </is>
+      </c>
+      <c r="J196" t="n">
+        <v>0.6933</v>
+      </c>
+      <c r="K196" t="n">
+        <v>0</v>
+      </c>
+      <c r="L196" t="n">
+        <v>0</v>
+      </c>
+      <c r="M196" t="n">
+        <v>170.72</v>
+      </c>
+      <c r="N196" t="inlineStr">
+        <is>
+          <t>[sl 0.69330]</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2026.01.26 10:03:58</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>705432349</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F197" t="n">
+        <v>5081.72</v>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>2026.01.26 22:03:24</t>
+        </is>
+      </c>
+      <c r="J197" t="n">
+        <v>5039.12</v>
+      </c>
+      <c r="K197" t="n">
+        <v>0</v>
+      </c>
+      <c r="L197" t="n">
+        <v>0</v>
+      </c>
+      <c r="M197" t="n">
+        <v>-852</v>
+      </c>
+      <c r="N197" t="inlineStr">
+        <is>
+          <t>[sl 5039.12]</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2026.01.27 11:16:10</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>711618843</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="F198" t="n">
+        <v>0.69097</v>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>2026.01.27 12:52:16</t>
+        </is>
+      </c>
+      <c r="J198" t="n">
+        <v>0.6923</v>
+      </c>
+      <c r="K198" t="n">
+        <v>0</v>
+      </c>
+      <c r="L198" t="n">
+        <v>0</v>
+      </c>
+      <c r="M198" t="n">
+        <v>-160.93</v>
+      </c>
+      <c r="N198" t="inlineStr">
+        <is>
+          <t>[sl 0.69230]</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2026.01.27 11:00:42</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>711565301</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="F199" t="n">
+        <v>5087.07</v>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>2026.01.27 23:53:54</t>
+        </is>
+      </c>
+      <c r="J199" t="n">
+        <v>5175.05</v>
+      </c>
+      <c r="K199" t="n">
+        <v>0</v>
+      </c>
+      <c r="L199" t="n">
+        <v>0</v>
+      </c>
+      <c r="M199" t="n">
+        <v>1231.72</v>
+      </c>
+      <c r="N199" t="inlineStr">
+        <is>
+          <t>[tp 5175.05]</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2026.01.28 11:24:38</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>717477122</v>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="F200" t="n">
+        <v>5292.2</v>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>2026.01.28 14:04:58</t>
+        </is>
+      </c>
+      <c r="J200" t="n">
+        <v>5247.96</v>
+      </c>
+      <c r="K200" t="n">
+        <v>0</v>
+      </c>
+      <c r="L200" t="n">
+        <v>0</v>
+      </c>
+      <c r="M200" t="n">
+        <v>-796.3200000000001</v>
+      </c>
+      <c r="N200" t="inlineStr">
+        <is>
+          <t>[sl 5247.96]</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2026.01.28 11:20:31</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>717465475</v>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F201" t="n">
+        <v>0.70081</v>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>2026.01.28 18:08:24</t>
+        </is>
+      </c>
+      <c r="J201" t="n">
+        <v>0.69809</v>
+      </c>
+      <c r="K201" t="n">
+        <v>0</v>
+      </c>
+      <c r="L201" t="n">
+        <v>0</v>
+      </c>
+      <c r="M201" t="n">
+        <v>-201.28</v>
+      </c>
+      <c r="N201" t="inlineStr">
+        <is>
+          <t>[sl 0.69809]</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2026.01.28 11:08:50</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>717422388</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F202" t="n">
+        <v>0.70029</v>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>2026.01.28 18:18:06</t>
+        </is>
+      </c>
+      <c r="J202" t="n">
+        <v>0.6976599999999999</v>
+      </c>
+      <c r="K202" t="n">
+        <v>0</v>
+      </c>
+      <c r="L202" t="n">
+        <v>0</v>
+      </c>
+      <c r="M202" t="n">
+        <v>-202.51</v>
+      </c>
+      <c r="N202" t="inlineStr">
+        <is>
+          <t>[sl 0.69766]</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2026.01.28 10:45:32</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>717319946</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>52.93</v>
+      </c>
+      <c r="F203" t="n">
+        <v>904.66</v>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>2026.01.29 05:49:44</t>
+        </is>
+      </c>
+      <c r="J203" t="n">
+        <v>893.0599999999999</v>
+      </c>
+      <c r="K203" t="n">
+        <v>0</v>
+      </c>
+      <c r="L203" t="n">
+        <v>-411.53</v>
+      </c>
+      <c r="M203" t="n">
+        <v>-6139.88</v>
+      </c>
+      <c r="N203" t="inlineStr">
+        <is>
+          <t>[sl 893.06]</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2026.01.29 11:08:58</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>725798101</v>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F204" t="n">
+        <v>0.70724</v>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>2026.01.29 13:36:24</t>
+        </is>
+      </c>
+      <c r="J204" t="n">
+        <v>0.7042</v>
+      </c>
+      <c r="K204" t="n">
+        <v>0</v>
+      </c>
+      <c r="L204" t="n">
+        <v>0</v>
+      </c>
+      <c r="M204" t="n">
+        <v>-170.24</v>
+      </c>
+      <c r="N204" t="inlineStr">
+        <is>
+          <t>[sl 0.70420]</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2026.01.29 11:02:33</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>725735954</v>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="F205" t="n">
+        <v>0.7071</v>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>2026.01.29 13:36:32</t>
+        </is>
+      </c>
+      <c r="J205" t="n">
+        <v>0.70414</v>
+      </c>
+      <c r="K205" t="n">
+        <v>0</v>
+      </c>
+      <c r="L205" t="n">
+        <v>0</v>
+      </c>
+      <c r="M205" t="n">
+        <v>-168.72</v>
+      </c>
+      <c r="N205" t="inlineStr">
+        <is>
+          <t>[sl 0.70414]</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2026.01.29 11:21:56</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>725882678</v>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F206" t="n">
+        <v>5538.16</v>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>2026.01.29 18:04:02</t>
+        </is>
+      </c>
+      <c r="J206" t="n">
+        <v>5446.12</v>
+      </c>
+      <c r="K206" t="n">
+        <v>0</v>
+      </c>
+      <c r="L206" t="n">
+        <v>0</v>
+      </c>
+      <c r="M206" t="n">
+        <v>-644.28</v>
+      </c>
+      <c r="N206" t="inlineStr">
+        <is>
+          <t>[sl 5446.12]</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2026.01.30 10:15:51</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>735345595</v>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>17.53</v>
+      </c>
+      <c r="F207" t="n">
+        <v>845.34</v>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>2026.01.30 10:31:48</t>
+        </is>
+      </c>
+      <c r="J207" t="n">
+        <v>844.84</v>
+      </c>
+      <c r="K207" t="n">
+        <v>0</v>
+      </c>
+      <c r="L207" t="n">
+        <v>0</v>
+      </c>
+      <c r="M207" t="n">
+        <v>87.65000000000001</v>
+      </c>
+      <c r="N207" t="inlineStr">
+        <is>
+          <t>[tp 844.84]</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2026.01.30 10:41:12</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>735524843</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E208" t="n">
+        <v>17.56</v>
+      </c>
+      <c r="F208" t="n">
+        <v>843.39</v>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>2026.01.30 11:34:48</t>
+        </is>
+      </c>
+      <c r="J208" t="n">
+        <v>842.89</v>
+      </c>
+      <c r="K208" t="n">
+        <v>0</v>
+      </c>
+      <c r="L208" t="n">
+        <v>0</v>
+      </c>
+      <c r="M208" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="N208" t="inlineStr">
+        <is>
+          <t>[tp 842.89]</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2026.01.30 11:48:12</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>736070754</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F209" t="n">
+        <v>5115.75</v>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>2026.01.30 12:57:22</t>
+        </is>
+      </c>
+      <c r="J209" t="n">
+        <v>5012.95</v>
+      </c>
+      <c r="K209" t="n">
+        <v>0</v>
+      </c>
+      <c r="L209" t="n">
+        <v>0</v>
+      </c>
+      <c r="M209" t="n">
+        <v>514</v>
+      </c>
+      <c r="N209" t="inlineStr">
+        <is>
+          <t>[sl 5012.95]</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2026.01.30 18:23:34</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>739230973</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="F210" t="n">
+        <v>6953.37</v>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>2026.01.30 19:21:17</t>
+        </is>
+      </c>
+      <c r="J210" t="n">
+        <v>6929.82</v>
+      </c>
+      <c r="K210" t="n">
+        <v>0</v>
+      </c>
+      <c r="L210" t="n">
+        <v>0</v>
+      </c>
+      <c r="M210" t="n">
+        <v>-993.8099999999999</v>
+      </c>
+      <c r="N210" t="inlineStr">
+        <is>
+          <t>[sl 6929.82]</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2026.02.01 10:00:57</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>743412751</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>17.09</v>
+      </c>
+      <c r="F211" t="n">
+        <v>775.98</v>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>2026.02.01 10:19:10</t>
+        </is>
+      </c>
+      <c r="J211" t="n">
+        <v>775.48</v>
+      </c>
+      <c r="K211" t="n">
+        <v>0</v>
+      </c>
+      <c r="L211" t="n">
+        <v>0</v>
+      </c>
+      <c r="M211" t="n">
+        <v>85.45</v>
+      </c>
+      <c r="N211" t="inlineStr">
+        <is>
+          <t>[tp 775.48]</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2026.02.01 10:39:02</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>743437269</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="F212" t="n">
+        <v>776.12</v>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>2026.02.01 13:37:41</t>
+        </is>
+      </c>
+      <c r="J212" t="n">
+        <v>775.63</v>
+      </c>
+      <c r="K212" t="n">
+        <v>0</v>
+      </c>
+      <c r="L212" t="n">
+        <v>0</v>
+      </c>
+      <c r="M212" t="n">
+        <v>78.98</v>
+      </c>
+      <c r="N212" t="inlineStr">
+        <is>
+          <t>[tp 775.63]</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2026.02.02 11:02:10</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>749086422</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="F213" t="n">
+        <v>6877.45</v>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>2026.02.02 11:02:12</t>
+        </is>
+      </c>
+      <c r="J213" t="n">
+        <v>6878.58</v>
+      </c>
+      <c r="K213" t="n">
+        <v>0</v>
+      </c>
+      <c r="L213" t="n">
+        <v>0</v>
+      </c>
+      <c r="M213" t="n">
+        <v>-52.66</v>
+      </c>
+      <c r="N213" t="inlineStr">
+        <is>
+          <t>[sl 6878.58]</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2026.02.02 11:04:08</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>749106194</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F214" t="n">
+        <v>4578.79</v>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>2026.02.02 14:40:22</t>
+        </is>
+      </c>
+      <c r="J214" t="n">
+        <v>4777.19</v>
+      </c>
+      <c r="K214" t="n">
+        <v>0</v>
+      </c>
+      <c r="L214" t="n">
+        <v>0</v>
+      </c>
+      <c r="M214" t="n">
+        <v>-595.2</v>
+      </c>
+      <c r="N214" t="inlineStr">
+        <is>
+          <t>[sl 4777.19]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour données 11 février 2026
</commit_message>
<xml_diff>
--- a/reports/ReportHistory-10960352.xlsx
+++ b/reports/ReportHistory-10960352.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N214"/>
+  <dimension ref="A1:N248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026.02.03 06:10</t>
+          <t>2026.02.11 06:10</t>
         </is>
       </c>
     </row>
@@ -10488,6 +10488,1638 @@
       <c r="N214" t="inlineStr">
         <is>
           <t>[sl 4777.19]</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2026.02.02 10:05:24</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>748594639</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>10.07</v>
+      </c>
+      <c r="F215" t="n">
+        <v>746.64</v>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>2026.02.03 21:19:38</t>
+        </is>
+      </c>
+      <c r="J215" t="n">
+        <v>746.14</v>
+      </c>
+      <c r="K215" t="n">
+        <v>0</v>
+      </c>
+      <c r="L215" t="n">
+        <v>-60.7</v>
+      </c>
+      <c r="M215" t="n">
+        <v>50.35</v>
+      </c>
+      <c r="N215" t="inlineStr">
+        <is>
+          <t>[tp 746.14]</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2026.02.03 21:27:40</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>762869715</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="F216" t="n">
+        <v>25227.47</v>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>2026.02.03 21:29:37</t>
+        </is>
+      </c>
+      <c r="J216" t="n">
+        <v>25221.32</v>
+      </c>
+      <c r="K216" t="n">
+        <v>0</v>
+      </c>
+      <c r="L216" t="n">
+        <v>0</v>
+      </c>
+      <c r="M216" t="n">
+        <v>156.83</v>
+      </c>
+      <c r="N216" t="inlineStr">
+        <is>
+          <t>[tp 25221.32]</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2026.02.03 21:16:39</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>762798041</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="F217" t="n">
+        <v>6895.96</v>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>2026.02.03 21:43:28</t>
+        </is>
+      </c>
+      <c r="J217" t="n">
+        <v>6884.07</v>
+      </c>
+      <c r="K217" t="n">
+        <v>0</v>
+      </c>
+      <c r="L217" t="n">
+        <v>0</v>
+      </c>
+      <c r="M217" t="n">
+        <v>469.66</v>
+      </c>
+      <c r="N217" t="inlineStr">
+        <is>
+          <t>closePosition</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2026.02.03 21:09:24</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>762760106</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F218" t="n">
+        <v>4941.22</v>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>2026.02.04 05:02:11</t>
+        </is>
+      </c>
+      <c r="J218" t="n">
+        <v>5059.26</v>
+      </c>
+      <c r="K218" t="n">
+        <v>0</v>
+      </c>
+      <c r="L218" t="n">
+        <v>-7.48</v>
+      </c>
+      <c r="M218" t="n">
+        <v>1062.36</v>
+      </c>
+      <c r="N218" t="inlineStr">
+        <is>
+          <t>[tp 5059.26]</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2026.02.04 13:02:34</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>767002514</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F219" t="n">
+        <v>754.35</v>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>2026.02.04 14:03:20</t>
+        </is>
+      </c>
+      <c r="J219" t="n">
+        <v>753.85</v>
+      </c>
+      <c r="K219" t="n">
+        <v>0</v>
+      </c>
+      <c r="L219" t="n">
+        <v>0</v>
+      </c>
+      <c r="M219" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N219" t="inlineStr">
+        <is>
+          <t>[tp 753.85]</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2026.02.04 11:13:25</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>766445054</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F220" t="n">
+        <v>5084.01</v>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>2026.02.04 14:17:33</t>
+        </is>
+      </c>
+      <c r="J220" t="n">
+        <v>5017.84</v>
+      </c>
+      <c r="K220" t="n">
+        <v>0</v>
+      </c>
+      <c r="L220" t="n">
+        <v>0</v>
+      </c>
+      <c r="M220" t="n">
+        <v>-529.36</v>
+      </c>
+      <c r="N220" t="inlineStr">
+        <is>
+          <t>[sl 5017.84]</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2026.02.04 15:29:31</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>767667721</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>10</v>
+      </c>
+      <c r="F221" t="n">
+        <v>25343.67</v>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>2026.02.04 16:34:55</t>
+        </is>
+      </c>
+      <c r="J221" t="n">
+        <v>25327.3</v>
+      </c>
+      <c r="K221" t="n">
+        <v>0</v>
+      </c>
+      <c r="L221" t="n">
+        <v>0</v>
+      </c>
+      <c r="M221" t="n">
+        <v>163.7</v>
+      </c>
+      <c r="N221" t="inlineStr">
+        <is>
+          <t>[sl 25327.30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2026.02.04 14:08:18</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>767288399</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F222" t="n">
+        <v>747.09</v>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>2026.02.04 16:41:39</t>
+        </is>
+      </c>
+      <c r="J222" t="n">
+        <v>746.59</v>
+      </c>
+      <c r="K222" t="n">
+        <v>0</v>
+      </c>
+      <c r="L222" t="n">
+        <v>0</v>
+      </c>
+      <c r="M222" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N222" t="inlineStr">
+        <is>
+          <t>[tp 746.59]</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2026.02.04 15:28:42</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>767664630</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F223" t="n">
+        <v>5049.98</v>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>2026.02.04 17:32:50</t>
+        </is>
+      </c>
+      <c r="J223" t="n">
+        <v>5007.53</v>
+      </c>
+      <c r="K223" t="n">
+        <v>0</v>
+      </c>
+      <c r="L223" t="n">
+        <v>0</v>
+      </c>
+      <c r="M223" t="n">
+        <v>-339.6</v>
+      </c>
+      <c r="N223" t="inlineStr">
+        <is>
+          <t>[sl 5007.53]</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2026.02.04 11:24:40</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>766492888</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>5</v>
+      </c>
+      <c r="F224" t="n">
+        <v>6928.91</v>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>2026.02.04 18:02:14</t>
+        </is>
+      </c>
+      <c r="J224" t="n">
+        <v>6891.95</v>
+      </c>
+      <c r="K224" t="n">
+        <v>0</v>
+      </c>
+      <c r="L224" t="n">
+        <v>0</v>
+      </c>
+      <c r="M224" t="n">
+        <v>184.8</v>
+      </c>
+      <c r="N224" t="inlineStr">
+        <is>
+          <t>[tp 6891.95]</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2026.02.05 11:46:28</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>775790482</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F225" t="n">
+        <v>4919.85</v>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>2026.02.05 12:45:47</t>
+        </is>
+      </c>
+      <c r="J225" t="n">
+        <v>4893.14</v>
+      </c>
+      <c r="K225" t="n">
+        <v>0</v>
+      </c>
+      <c r="L225" t="n">
+        <v>0</v>
+      </c>
+      <c r="M225" t="n">
+        <v>186.97</v>
+      </c>
+      <c r="N225" t="inlineStr">
+        <is>
+          <t>[sl 4893.14]</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2026.02.05 14:44:31</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>776966685</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>2</v>
+      </c>
+      <c r="F226" t="n">
+        <v>685.64</v>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>2026.02.05 14:47:14</t>
+        </is>
+      </c>
+      <c r="J226" t="n">
+        <v>685.14</v>
+      </c>
+      <c r="K226" t="n">
+        <v>0</v>
+      </c>
+      <c r="L226" t="n">
+        <v>0</v>
+      </c>
+      <c r="M226" t="n">
+        <v>10</v>
+      </c>
+      <c r="N226" t="inlineStr">
+        <is>
+          <t>[tp 685.14]</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2026.02.05 15:01:23</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>777075437</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>2</v>
+      </c>
+      <c r="F227" t="n">
+        <v>682.8200000000001</v>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>2026.02.05 15:15:44</t>
+        </is>
+      </c>
+      <c r="J227" t="n">
+        <v>682.3200000000001</v>
+      </c>
+      <c r="K227" t="n">
+        <v>0</v>
+      </c>
+      <c r="L227" t="n">
+        <v>0</v>
+      </c>
+      <c r="M227" t="n">
+        <v>10</v>
+      </c>
+      <c r="N227" t="inlineStr">
+        <is>
+          <t>[tp 682.32]</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2026.02.05 15:17:57</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>777224852</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F228" t="n">
+        <v>24934.12</v>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>2026.02.05 15:18:00</t>
+        </is>
+      </c>
+      <c r="J228" t="n">
+        <v>24933.62</v>
+      </c>
+      <c r="K228" t="n">
+        <v>0</v>
+      </c>
+      <c r="L228" t="n">
+        <v>0</v>
+      </c>
+      <c r="M228" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="N228" t="inlineStr">
+        <is>
+          <t>[tp 24933.62]</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2026.02.05 15:23:55</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>777282330</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="F229" t="n">
+        <v>24819.87</v>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>2026.02.05 15:33:17</t>
+        </is>
+      </c>
+      <c r="J229" t="n">
+        <v>24777.98</v>
+      </c>
+      <c r="K229" t="n">
+        <v>0</v>
+      </c>
+      <c r="L229" t="n">
+        <v>0</v>
+      </c>
+      <c r="M229" t="n">
+        <v>410.52</v>
+      </c>
+      <c r="N229" t="inlineStr">
+        <is>
+          <t>[tp 24777.98]</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2026.02.05 15:13:53</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>777186834</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E230" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F230" t="n">
+        <v>4836.21</v>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>2026.02.05 16:06:35</t>
+        </is>
+      </c>
+      <c r="J230" t="n">
+        <v>4807.44</v>
+      </c>
+      <c r="K230" t="n">
+        <v>0</v>
+      </c>
+      <c r="L230" t="n">
+        <v>0</v>
+      </c>
+      <c r="M230" t="n">
+        <v>230.16</v>
+      </c>
+      <c r="N230" t="inlineStr">
+        <is>
+          <t>[tp 4807.44]</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2026.02.06 11:26:58</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>785631058</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E231" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F231" t="n">
+        <v>4866.69</v>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>2026.02.06 11:31:09</t>
+        </is>
+      </c>
+      <c r="J231" t="n">
+        <v>4874.75</v>
+      </c>
+      <c r="K231" t="n">
+        <v>0</v>
+      </c>
+      <c r="L231" t="n">
+        <v>0</v>
+      </c>
+      <c r="M231" t="n">
+        <v>64.48</v>
+      </c>
+      <c r="N231" t="inlineStr">
+        <is>
+          <t>[tp 4874.75]</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2026.02.06 15:09:42</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>786741799</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E232" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F232" t="n">
+        <v>4901.85</v>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>2026.02.06 15:21:47</t>
+        </is>
+      </c>
+      <c r="J232" t="n">
+        <v>4878.73</v>
+      </c>
+      <c r="K232" t="n">
+        <v>0</v>
+      </c>
+      <c r="L232" t="n">
+        <v>0</v>
+      </c>
+      <c r="M232" t="n">
+        <v>-184.96</v>
+      </c>
+      <c r="N232" t="inlineStr">
+        <is>
+          <t>[sl 4878.73]</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2026.02.06 11:26:07</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>785626224</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E233" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F233" t="n">
+        <v>0.69638</v>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>2026.02.06 16:37:46</t>
+        </is>
+      </c>
+      <c r="J233" t="n">
+        <v>0.69869</v>
+      </c>
+      <c r="K233" t="n">
+        <v>0</v>
+      </c>
+      <c r="L233" t="n">
+        <v>0</v>
+      </c>
+      <c r="M233" t="n">
+        <v>164.01</v>
+      </c>
+      <c r="N233" t="inlineStr">
+        <is>
+          <t>[sl 0.69869]</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2026.02.06 15:01:35</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>786694501</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E234" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F234" t="n">
+        <v>0.69854</v>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>2026.02.06 17:55:29</t>
+        </is>
+      </c>
+      <c r="J234" t="n">
+        <v>0.70042</v>
+      </c>
+      <c r="K234" t="n">
+        <v>0</v>
+      </c>
+      <c r="L234" t="n">
+        <v>0</v>
+      </c>
+      <c r="M234" t="n">
+        <v>144.76</v>
+      </c>
+      <c r="N234" t="inlineStr">
+        <is>
+          <t>[sl 0.70042]</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2026.02.06 18:15:59</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>788072420</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E235" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="F235" t="n">
+        <v>24695.22</v>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>2026.02.06 18:16:00</t>
+        </is>
+      </c>
+      <c r="J235" t="n">
+        <v>24693.97</v>
+      </c>
+      <c r="K235" t="n">
+        <v>0</v>
+      </c>
+      <c r="L235" t="n">
+        <v>0</v>
+      </c>
+      <c r="M235" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="N235" t="inlineStr">
+        <is>
+          <t>[tp 24693.97]</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2026.02.06 14:01:03</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>786406520</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E236" t="n">
+        <v>2</v>
+      </c>
+      <c r="F236" t="n">
+        <v>631.09</v>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>2026.02.09 11:22:26</t>
+        </is>
+      </c>
+      <c r="J236" t="n">
+        <v>630.59</v>
+      </c>
+      <c r="K236" t="n">
+        <v>0</v>
+      </c>
+      <c r="L236" t="n">
+        <v>-12.16</v>
+      </c>
+      <c r="M236" t="n">
+        <v>10</v>
+      </c>
+      <c r="N236" t="inlineStr">
+        <is>
+          <t>[tp 630.59]</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2026.02.09 15:24:34</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>796894058</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E237" t="n">
+        <v>5</v>
+      </c>
+      <c r="F237" t="n">
+        <v>6925.11</v>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>2026.02.09 16:06:37</t>
+        </is>
+      </c>
+      <c r="J237" t="n">
+        <v>6934.68</v>
+      </c>
+      <c r="K237" t="n">
+        <v>0</v>
+      </c>
+      <c r="L237" t="n">
+        <v>0</v>
+      </c>
+      <c r="M237" t="n">
+        <v>47.85</v>
+      </c>
+      <c r="N237" t="inlineStr">
+        <is>
+          <t>[tp 6934.68]</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2026.02.09 14:28:11</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>796622929</v>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>LTCUSD</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E238" t="n">
+        <v>1</v>
+      </c>
+      <c r="F238" t="n">
+        <v>52.36</v>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>2026.02.09 17:40:17</t>
+        </is>
+      </c>
+      <c r="J238" t="n">
+        <v>54.56</v>
+      </c>
+      <c r="K238" t="n">
+        <v>0</v>
+      </c>
+      <c r="L238" t="n">
+        <v>0</v>
+      </c>
+      <c r="M238" t="n">
+        <v>-220</v>
+      </c>
+      <c r="N238" t="inlineStr">
+        <is>
+          <t>[sl 54.56]</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2026.02.09 18:07:44</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>797984600</v>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E239" t="n">
+        <v>10</v>
+      </c>
+      <c r="F239" t="n">
+        <v>25132.25</v>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>2026.02.09 18:07:45</t>
+        </is>
+      </c>
+      <c r="J239" t="n">
+        <v>25132.75</v>
+      </c>
+      <c r="K239" t="n">
+        <v>0</v>
+      </c>
+      <c r="L239" t="n">
+        <v>0</v>
+      </c>
+      <c r="M239" t="n">
+        <v>5</v>
+      </c>
+      <c r="N239" t="inlineStr">
+        <is>
+          <t>[tp 25132.75]</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2026.02.09 18:08:42</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>797990610</v>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E240" t="n">
+        <v>5</v>
+      </c>
+      <c r="F240" t="n">
+        <v>6942.11</v>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>2026.02.09 18:19:32</t>
+        </is>
+      </c>
+      <c r="J240" t="n">
+        <v>6950.72</v>
+      </c>
+      <c r="K240" t="n">
+        <v>0</v>
+      </c>
+      <c r="L240" t="n">
+        <v>0</v>
+      </c>
+      <c r="M240" t="n">
+        <v>43.05</v>
+      </c>
+      <c r="N240" t="inlineStr">
+        <is>
+          <t>[tp 6950.72]</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2026.02.09 16:44:39</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>797387426</v>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E241" t="n">
+        <v>2</v>
+      </c>
+      <c r="F241" t="n">
+        <v>626.97</v>
+      </c>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>2026.02.09 23:08:53</t>
+        </is>
+      </c>
+      <c r="J241" t="n">
+        <v>645.4</v>
+      </c>
+      <c r="K241" t="n">
+        <v>0</v>
+      </c>
+      <c r="L241" t="n">
+        <v>0</v>
+      </c>
+      <c r="M241" t="n">
+        <v>-368.6</v>
+      </c>
+      <c r="N241" t="inlineStr">
+        <is>
+          <t>[sl 645.40]</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2026.02.10 15:05:00</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>803334704</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E242" t="n">
+        <v>10</v>
+      </c>
+      <c r="F242" t="n">
+        <v>25320.95</v>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>2026.02.10 15:25:52</t>
+        </is>
+      </c>
+      <c r="J242" t="n">
+        <v>25337.56</v>
+      </c>
+      <c r="K242" t="n">
+        <v>0</v>
+      </c>
+      <c r="L242" t="n">
+        <v>0</v>
+      </c>
+      <c r="M242" t="n">
+        <v>166.1</v>
+      </c>
+      <c r="N242" t="inlineStr">
+        <is>
+          <t>[tp 25337.56]</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2026.02.10 15:04:39</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>803332393</v>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E243" t="n">
+        <v>5</v>
+      </c>
+      <c r="F243" t="n">
+        <v>6978.26</v>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>2026.02.10 15:41:00</t>
+        </is>
+      </c>
+      <c r="J243" t="n">
+        <v>6967.93</v>
+      </c>
+      <c r="K243" t="n">
+        <v>0</v>
+      </c>
+      <c r="L243" t="n">
+        <v>0</v>
+      </c>
+      <c r="M243" t="n">
+        <v>-51.65</v>
+      </c>
+      <c r="N243" t="inlineStr">
+        <is>
+          <t>[sl 6967.93]</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2026.02.10 11:32:59</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>802379508</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E244" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="F244" t="n">
+        <v>0.7073700000000001</v>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>2026.02.10 17:37:26</t>
+        </is>
+      </c>
+      <c r="J244" t="n">
+        <v>0.70822</v>
+      </c>
+      <c r="K244" t="n">
+        <v>0</v>
+      </c>
+      <c r="L244" t="n">
+        <v>0</v>
+      </c>
+      <c r="M244" t="n">
+        <v>95.2</v>
+      </c>
+      <c r="N244" t="inlineStr">
+        <is>
+          <t>[sl 0.70822]</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2026.02.10 11:53:23</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>802483563</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E245" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="F245" t="n">
+        <v>0.70733</v>
+      </c>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>2026.02.10 17:37:26</t>
+        </is>
+      </c>
+      <c r="J245" t="n">
+        <v>0.70822</v>
+      </c>
+      <c r="K245" t="n">
+        <v>0</v>
+      </c>
+      <c r="L245" t="n">
+        <v>0</v>
+      </c>
+      <c r="M245" t="n">
+        <v>99.68000000000001</v>
+      </c>
+      <c r="N245" t="inlineStr">
+        <is>
+          <t>[sl 0.70822]</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2026.02.10 18:10:18</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>804605665</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E246" t="n">
+        <v>10</v>
+      </c>
+      <c r="F246" t="n">
+        <v>25367.7</v>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>2026.02.10 18:10:36</t>
+        </is>
+      </c>
+      <c r="J246" t="n">
+        <v>25368.2</v>
+      </c>
+      <c r="K246" t="n">
+        <v>0</v>
+      </c>
+      <c r="L246" t="n">
+        <v>0</v>
+      </c>
+      <c r="M246" t="n">
+        <v>5</v>
+      </c>
+      <c r="N246" t="inlineStr">
+        <is>
+          <t>[tp 25368.20]</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2026.02.10 18:00:06</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>804520611</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E247" t="n">
+        <v>5</v>
+      </c>
+      <c r="F247" t="n">
+        <v>6981.26</v>
+      </c>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>2026.02.10 21:52:00</t>
+        </is>
+      </c>
+      <c r="J247" t="n">
+        <v>6953.44</v>
+      </c>
+      <c r="K247" t="n">
+        <v>0</v>
+      </c>
+      <c r="L247" t="n">
+        <v>0</v>
+      </c>
+      <c r="M247" t="n">
+        <v>-139.1</v>
+      </c>
+      <c r="N247" t="inlineStr">
+        <is>
+          <t>[sl 6953.44]</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2026.02.09 18:09:21</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>797994916</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E248" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F248" t="n">
+        <v>0.70821</v>
+      </c>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>2026.02.11 05:32:42</t>
+        </is>
+      </c>
+      <c r="J248" t="n">
+        <v>0.71171</v>
+      </c>
+      <c r="K248" t="n">
+        <v>0</v>
+      </c>
+      <c r="L248" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="M248" t="n">
+        <v>262.5</v>
+      </c>
+      <c r="N248" t="inlineStr">
+        <is>
+          <t>[tp 0.71171]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour données 12 février 2026
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/reports/ReportHistory-10960352.xlsx
+++ b/reports/ReportHistory-10960352.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N248"/>
+  <dimension ref="A1:N260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026.02.11 06:10</t>
+          <t>2026.02.13 06:10</t>
         </is>
       </c>
     </row>
@@ -12120,6 +12120,582 @@
       <c r="N248" t="inlineStr">
         <is>
           <t>[tp 0.71171]</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2026.02.11 15:22:01</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>809278101</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E249" t="n">
+        <v>10</v>
+      </c>
+      <c r="F249" t="n">
+        <v>25194.5</v>
+      </c>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>2026.02.11 16:30:01</t>
+        </is>
+      </c>
+      <c r="J249" t="n">
+        <v>25238.19</v>
+      </c>
+      <c r="K249" t="n">
+        <v>0</v>
+      </c>
+      <c r="L249" t="n">
+        <v>0</v>
+      </c>
+      <c r="M249" t="n">
+        <v>436.9</v>
+      </c>
+      <c r="N249" t="inlineStr">
+        <is>
+          <t>[tp 25238.19]</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2026.02.11 11:05:54</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>808191793</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E250" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F250" t="n">
+        <v>0.71094</v>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>2026.02.11 16:30:02</t>
+        </is>
+      </c>
+      <c r="J250" t="n">
+        <v>0.70896</v>
+      </c>
+      <c r="K250" t="n">
+        <v>0</v>
+      </c>
+      <c r="L250" t="n">
+        <v>0</v>
+      </c>
+      <c r="M250" t="n">
+        <v>-168.3</v>
+      </c>
+      <c r="N250" t="inlineStr">
+        <is>
+          <t>[sl 0.70896]</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2026.02.11 11:40:20</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>808309734</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E251" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="F251" t="n">
+        <v>0.7105399999999999</v>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>2026.02.11 16:30:08</t>
+        </is>
+      </c>
+      <c r="J251" t="n">
+        <v>0.70849</v>
+      </c>
+      <c r="K251" t="n">
+        <v>0</v>
+      </c>
+      <c r="L251" t="n">
+        <v>0</v>
+      </c>
+      <c r="M251" t="n">
+        <v>-168.1</v>
+      </c>
+      <c r="N251" t="inlineStr">
+        <is>
+          <t>[sl 0.70849]</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2026.02.11 15:11:55</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>809225290</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E252" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="F252" t="n">
+        <v>25194.25</v>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>2026.02.11 16:46:12</t>
+        </is>
+      </c>
+      <c r="J252" t="n">
+        <v>25307.24</v>
+      </c>
+      <c r="K252" t="n">
+        <v>0</v>
+      </c>
+      <c r="L252" t="n">
+        <v>0</v>
+      </c>
+      <c r="M252" t="n">
+        <v>983.01</v>
+      </c>
+      <c r="N252" t="inlineStr">
+        <is>
+          <t>[tp 25307.24]</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2026.02.11 11:30:28</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>808265079</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>LTCUSD</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E253" t="n">
+        <v>1</v>
+      </c>
+      <c r="F253" t="n">
+        <v>51.38</v>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>2026.02.11 17:02:52</t>
+        </is>
+      </c>
+      <c r="J253" t="n">
+        <v>53.28</v>
+      </c>
+      <c r="K253" t="n">
+        <v>0</v>
+      </c>
+      <c r="L253" t="n">
+        <v>0</v>
+      </c>
+      <c r="M253" t="n">
+        <v>-190</v>
+      </c>
+      <c r="N253" t="inlineStr">
+        <is>
+          <t>[sl 53.28]</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2026.02.11 18:35:58</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>810945618</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E254" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="F254" t="n">
+        <v>25081.32</v>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>2026.02.11 23:30:40</t>
+        </is>
+      </c>
+      <c r="J254" t="n">
+        <v>25208</v>
+      </c>
+      <c r="K254" t="n">
+        <v>0</v>
+      </c>
+      <c r="L254" t="n">
+        <v>0</v>
+      </c>
+      <c r="M254" t="n">
+        <v>-1038.78</v>
+      </c>
+      <c r="N254" t="inlineStr">
+        <is>
+          <t>close_before_mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2026.02.12 09:18:57</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>814015047</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E255" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="F255" t="n">
+        <v>67135.66</v>
+      </c>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>2026.02.12 09:19:28</t>
+        </is>
+      </c>
+      <c r="J255" t="n">
+        <v>67135.16</v>
+      </c>
+      <c r="K255" t="n">
+        <v>0</v>
+      </c>
+      <c r="L255" t="n">
+        <v>0</v>
+      </c>
+      <c r="M255" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="N255" t="inlineStr">
+        <is>
+          <t>[tp 67135.16]</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2026.02.12 09:35:59</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>814090386</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E256" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="F256" t="n">
+        <v>67178.98</v>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>2026.02.12 09:36:00</t>
+        </is>
+      </c>
+      <c r="J256" t="n">
+        <v>67184.03999999999</v>
+      </c>
+      <c r="K256" t="n">
+        <v>0</v>
+      </c>
+      <c r="L256" t="n">
+        <v>0</v>
+      </c>
+      <c r="M256" t="n">
+        <v>-2.43</v>
+      </c>
+      <c r="N256" t="inlineStr">
+        <is>
+          <t>[tp 67184.04]</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2026.02.12 11:01:13</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>814382898</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E257" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F257" t="n">
+        <v>5064.66</v>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>2026.02.12 17:04:05</t>
+        </is>
+      </c>
+      <c r="J257" t="n">
+        <v>5071.43</v>
+      </c>
+      <c r="K257" t="n">
+        <v>0</v>
+      </c>
+      <c r="L257" t="n">
+        <v>0</v>
+      </c>
+      <c r="M257" t="n">
+        <v>54.16</v>
+      </c>
+      <c r="N257" t="inlineStr">
+        <is>
+          <t>[sl 5071.43]</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2026.02.12 15:35:12</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>815389911</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E258" t="n">
+        <v>10</v>
+      </c>
+      <c r="F258" t="n">
+        <v>25303.75</v>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>2026.02.12 17:44:10</t>
+        </is>
+      </c>
+      <c r="J258" t="n">
+        <v>25250.92</v>
+      </c>
+      <c r="K258" t="n">
+        <v>0</v>
+      </c>
+      <c r="L258" t="n">
+        <v>0</v>
+      </c>
+      <c r="M258" t="n">
+        <v>-528.3</v>
+      </c>
+      <c r="N258" t="inlineStr">
+        <is>
+          <t>[sl 25250.92]</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2026.02.12 11:08:36</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>814416556</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E259" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="F259" t="n">
+        <v>0.71223</v>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>2026.02.12 19:15:43</t>
+        </is>
+      </c>
+      <c r="J259" t="n">
+        <v>0.71008</v>
+      </c>
+      <c r="K259" t="n">
+        <v>0</v>
+      </c>
+      <c r="L259" t="n">
+        <v>0</v>
+      </c>
+      <c r="M259" t="n">
+        <v>-174.15</v>
+      </c>
+      <c r="N259" t="inlineStr">
+        <is>
+          <t>[sl 0.71008]</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2026.02.12 11:00:13</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>814378525</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E260" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F260" t="n">
+        <v>0.71216</v>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>2026.02.12 19:16:17</t>
+        </is>
+      </c>
+      <c r="J260" t="n">
+        <v>0.70987</v>
+      </c>
+      <c r="K260" t="n">
+        <v>0</v>
+      </c>
+      <c r="L260" t="n">
+        <v>0</v>
+      </c>
+      <c r="M260" t="n">
+        <v>-174.04</v>
+      </c>
+      <c r="N260" t="inlineStr">
+        <is>
+          <t>[sl 0.70987]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour données 20 février 2026
- deals_history, equity_log, proposals_log, trades_log
- Journaux de trading du 13 au 19 février 2026
- Sentiment cache (9 symboles)
- Performance tracker, pm_state, open_positions
- News calendar + rapport ReportHistory

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/reports/ReportHistory-10960352.xlsx
+++ b/reports/ReportHistory-10960352.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N260"/>
+  <dimension ref="A1:N295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026.02.13 06:10</t>
+          <t>2026.02.20 06:10</t>
         </is>
       </c>
     </row>
@@ -12696,6 +12696,1686 @@
       <c r="N260" t="inlineStr">
         <is>
           <t>[sl 0.70987]</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2026.02.13 09:02:39</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>820855234</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E261" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F261" t="n">
+        <v>66218.98</v>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>2026.02.13 09:51:49</t>
+        </is>
+      </c>
+      <c r="J261" t="n">
+        <v>66218.98</v>
+      </c>
+      <c r="K261" t="n">
+        <v>0</v>
+      </c>
+      <c r="L261" t="n">
+        <v>0</v>
+      </c>
+      <c r="M261" t="n">
+        <v>0</v>
+      </c>
+      <c r="N261" t="inlineStr">
+        <is>
+          <t>[sl 66218.98]</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2026.02.13 13:13:58</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>822103634</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E262" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F262" t="n">
+        <v>66863.22</v>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>2026.02.13 16:39:26</t>
+        </is>
+      </c>
+      <c r="J262" t="n">
+        <v>67254.02</v>
+      </c>
+      <c r="K262" t="n">
+        <v>0</v>
+      </c>
+      <c r="L262" t="n">
+        <v>0</v>
+      </c>
+      <c r="M262" t="n">
+        <v>195.4</v>
+      </c>
+      <c r="N262" t="inlineStr">
+        <is>
+          <t>[sl 67254.02]</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2026.02.13 18:03:31</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>824128326</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E263" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F263" t="n">
+        <v>5000.82</v>
+      </c>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>2026.02.13 18:08:04</t>
+        </is>
+      </c>
+      <c r="J263" t="n">
+        <v>5007.39</v>
+      </c>
+      <c r="K263" t="n">
+        <v>0</v>
+      </c>
+      <c r="L263" t="n">
+        <v>0</v>
+      </c>
+      <c r="M263" t="n">
+        <v>52.56</v>
+      </c>
+      <c r="N263" t="inlineStr">
+        <is>
+          <t>[tp 5007.39]</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2026.02.13 10:02:30</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>821145107</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E264" t="n">
+        <v>2</v>
+      </c>
+      <c r="F264" t="n">
+        <v>596.1</v>
+      </c>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>2026.02.13 18:26:34</t>
+        </is>
+      </c>
+      <c r="J264" t="n">
+        <v>611.23</v>
+      </c>
+      <c r="K264" t="n">
+        <v>0</v>
+      </c>
+      <c r="L264" t="n">
+        <v>0</v>
+      </c>
+      <c r="M264" t="n">
+        <v>-302.6</v>
+      </c>
+      <c r="N264" t="inlineStr">
+        <is>
+          <t>[sl 611.23]</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2026.02.13 18:21:04</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>824319638</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E265" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F265" t="n">
+        <v>4998.42</v>
+      </c>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>2026.02.13 18:27:53</t>
+        </is>
+      </c>
+      <c r="J265" t="n">
+        <v>5007.39</v>
+      </c>
+      <c r="K265" t="n">
+        <v>0</v>
+      </c>
+      <c r="L265" t="n">
+        <v>0</v>
+      </c>
+      <c r="M265" t="n">
+        <v>71.76000000000001</v>
+      </c>
+      <c r="N265" t="inlineStr">
+        <is>
+          <t>[tp 5007.39]</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2026.02.13 18:46:06</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>824546093</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E266" t="n">
+        <v>5</v>
+      </c>
+      <c r="F266" t="n">
+        <v>6837.55</v>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>2026.02.13 18:46:23</t>
+        </is>
+      </c>
+      <c r="J266" t="n">
+        <v>6836.8</v>
+      </c>
+      <c r="K266" t="n">
+        <v>0</v>
+      </c>
+      <c r="L266" t="n">
+        <v>0</v>
+      </c>
+      <c r="M266" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="N266" t="inlineStr">
+        <is>
+          <t>[tp 6836.80]</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2026.02.14 12:15:50</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>826398389</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E267" t="n">
+        <v>2</v>
+      </c>
+      <c r="F267" t="n">
+        <v>627.7</v>
+      </c>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>2026.02.14 14:10:29</t>
+        </is>
+      </c>
+      <c r="J267" t="n">
+        <v>628.2</v>
+      </c>
+      <c r="K267" t="n">
+        <v>0</v>
+      </c>
+      <c r="L267" t="n">
+        <v>0</v>
+      </c>
+      <c r="M267" t="n">
+        <v>10</v>
+      </c>
+      <c r="N267" t="inlineStr">
+        <is>
+          <t>[tp 628.20]</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2026.02.14 16:35:20</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>826614473</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>SOLUSD</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E268" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="F268" t="n">
+        <v>86.53</v>
+      </c>
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>2026.02.14 19:44:29</t>
+        </is>
+      </c>
+      <c r="J268" t="n">
+        <v>87.7</v>
+      </c>
+      <c r="K268" t="n">
+        <v>0</v>
+      </c>
+      <c r="L268" t="n">
+        <v>0</v>
+      </c>
+      <c r="M268" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="N268" t="inlineStr">
+        <is>
+          <t>[tp 87.70]</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2026.02.14 09:31:26</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>826300184</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E269" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="F269" t="n">
+        <v>68902.95</v>
+      </c>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>2026.02.15 11:29:07</t>
+        </is>
+      </c>
+      <c r="J269" t="n">
+        <v>70575.35000000001</v>
+      </c>
+      <c r="K269" t="n">
+        <v>0</v>
+      </c>
+      <c r="L269" t="n">
+        <v>0</v>
+      </c>
+      <c r="M269" t="n">
+        <v>518.45</v>
+      </c>
+      <c r="N269" t="inlineStr">
+        <is>
+          <t>[sl 70575.35]</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2026.02.15 11:54:33</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>827440317</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E270" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F270" t="n">
+        <v>70438.14999999999</v>
+      </c>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>2026.02.15 16:29:04</t>
+        </is>
+      </c>
+      <c r="J270" t="n">
+        <v>69172.14</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0</v>
+      </c>
+      <c r="L270" t="n">
+        <v>0</v>
+      </c>
+      <c r="M270" t="n">
+        <v>-633.01</v>
+      </c>
+      <c r="N270" t="inlineStr">
+        <is>
+          <t>[sl 69172.14]</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2026.02.15 16:31:06</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>827727886</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E271" t="n">
+        <v>2</v>
+      </c>
+      <c r="F271" t="n">
+        <v>618.6900000000001</v>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>2026.02.15 20:45:03</t>
+        </is>
+      </c>
+      <c r="J271" t="n">
+        <v>615.9400000000001</v>
+      </c>
+      <c r="K271" t="n">
+        <v>0</v>
+      </c>
+      <c r="L271" t="n">
+        <v>0</v>
+      </c>
+      <c r="M271" t="n">
+        <v>55</v>
+      </c>
+      <c r="N271" t="inlineStr">
+        <is>
+          <t>[tp 615.94]</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2026.02.16 11:53:05</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>830233868</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E272" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F272" t="n">
+        <v>0.70943</v>
+      </c>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>2026.02.16 14:11:57</t>
+        </is>
+      </c>
+      <c r="J272" t="n">
+        <v>0.7078</v>
+      </c>
+      <c r="K272" t="n">
+        <v>0</v>
+      </c>
+      <c r="L272" t="n">
+        <v>0</v>
+      </c>
+      <c r="M272" t="n">
+        <v>-161.37</v>
+      </c>
+      <c r="N272" t="inlineStr">
+        <is>
+          <t>[sl 0.70780]</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2026.02.16 12:37:34</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>830382092</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E273" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F273" t="n">
+        <v>69017.28999999999</v>
+      </c>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>2026.02.16 16:01:41</t>
+        </is>
+      </c>
+      <c r="J273" t="n">
+        <v>69852.03</v>
+      </c>
+      <c r="K273" t="n">
+        <v>0</v>
+      </c>
+      <c r="L273" t="n">
+        <v>0</v>
+      </c>
+      <c r="M273" t="n">
+        <v>417.37</v>
+      </c>
+      <c r="N273" t="inlineStr">
+        <is>
+          <t>[tp 69852.03]</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2026.02.16 15:21:56</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>830968295</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E274" t="n">
+        <v>5</v>
+      </c>
+      <c r="F274" t="n">
+        <v>6863.11</v>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>2026.02.16 17:14:25</t>
+        </is>
+      </c>
+      <c r="J274" t="n">
+        <v>6849.94</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0</v>
+      </c>
+      <c r="L274" t="n">
+        <v>0</v>
+      </c>
+      <c r="M274" t="n">
+        <v>-65.84999999999999</v>
+      </c>
+      <c r="N274" t="inlineStr">
+        <is>
+          <t>[sl 6849.94]</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2026.02.16 11:03:24</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>830034066</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E275" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="F275" t="n">
+        <v>0.7088100000000001</v>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>2026.02.16 17:45:25</t>
+        </is>
+      </c>
+      <c r="J275" t="n">
+        <v>0.7073700000000001</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0</v>
+      </c>
+      <c r="L275" t="n">
+        <v>0</v>
+      </c>
+      <c r="M275" t="n">
+        <v>-152.64</v>
+      </c>
+      <c r="N275" t="inlineStr">
+        <is>
+          <t>[sl 0.70737]</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2026.02.16 16:33:00</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>831275501</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>SOLUSD</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E276" t="n">
+        <v>1</v>
+      </c>
+      <c r="F276" t="n">
+        <v>84.76000000000001</v>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>2026.02.16 18:31:37</t>
+        </is>
+      </c>
+      <c r="J276" t="n">
+        <v>83.41</v>
+      </c>
+      <c r="K276" t="n">
+        <v>0</v>
+      </c>
+      <c r="L276" t="n">
+        <v>0</v>
+      </c>
+      <c r="M276" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="N276" t="inlineStr">
+        <is>
+          <t>[tp 83.41]</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2026.02.16 11:04:23</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>830040677</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E277" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F277" t="n">
+        <v>5011.65</v>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>2026.02.17 03:52:15</t>
+        </is>
+      </c>
+      <c r="J277" t="n">
+        <v>4965.25</v>
+      </c>
+      <c r="K277" t="n">
+        <v>0</v>
+      </c>
+      <c r="L277" t="n">
+        <v>-19.43</v>
+      </c>
+      <c r="M277" t="n">
+        <v>-928</v>
+      </c>
+      <c r="N277" t="inlineStr">
+        <is>
+          <t>[sl 4965.25]</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2026.02.17 12:14:55</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>835256561</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E278" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F278" t="n">
+        <v>68098.08</v>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>2026.02.17 13:16:17</t>
+        </is>
+      </c>
+      <c r="J278" t="n">
+        <v>67956.53</v>
+      </c>
+      <c r="K278" t="n">
+        <v>0</v>
+      </c>
+      <c r="L278" t="n">
+        <v>0</v>
+      </c>
+      <c r="M278" t="n">
+        <v>70.77</v>
+      </c>
+      <c r="N278" t="inlineStr">
+        <is>
+          <t>[tp 67956.53]</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2026.02.17 13:24:31</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>835567708</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E279" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F279" t="n">
+        <v>67935.12</v>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>2026.02.17 14:21:18</t>
+        </is>
+      </c>
+      <c r="J279" t="n">
+        <v>67935.12</v>
+      </c>
+      <c r="K279" t="n">
+        <v>0</v>
+      </c>
+      <c r="L279" t="n">
+        <v>0</v>
+      </c>
+      <c r="M279" t="n">
+        <v>0</v>
+      </c>
+      <c r="N279" t="inlineStr">
+        <is>
+          <t>[sl 67935.12]</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2026.02.17 18:14:56</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>837578784</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>USDJPY</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E280" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F280" t="n">
+        <v>153.608</v>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>2026.02.17 18:45:59</t>
+        </is>
+      </c>
+      <c r="J280" t="n">
+        <v>153.904</v>
+      </c>
+      <c r="K280" t="n">
+        <v>0</v>
+      </c>
+      <c r="L280" t="n">
+        <v>0</v>
+      </c>
+      <c r="M280" t="n">
+        <v>134.63</v>
+      </c>
+      <c r="N280" t="inlineStr">
+        <is>
+          <t>[tp 153.904]</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2026.02.17 18:10:42</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>837539206</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E281" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F281" t="n">
+        <v>0.7039800000000001</v>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>2026.02.17 19:15:35</t>
+        </is>
+      </c>
+      <c r="J281" t="n">
+        <v>0.70595</v>
+      </c>
+      <c r="K281" t="n">
+        <v>0</v>
+      </c>
+      <c r="L281" t="n">
+        <v>0</v>
+      </c>
+      <c r="M281" t="n">
+        <v>-157.6</v>
+      </c>
+      <c r="N281" t="inlineStr">
+        <is>
+          <t>[sl 0.70595]</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2026.02.17 18:01:49</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>837453021</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E282" t="n">
+        <v>5</v>
+      </c>
+      <c r="F282" t="n">
+        <v>6793.8</v>
+      </c>
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>2026.02.17 21:39:54</t>
+        </is>
+      </c>
+      <c r="J282" t="n">
+        <v>6855.85</v>
+      </c>
+      <c r="K282" t="n">
+        <v>0</v>
+      </c>
+      <c r="L282" t="n">
+        <v>0</v>
+      </c>
+      <c r="M282" t="n">
+        <v>-310.25</v>
+      </c>
+      <c r="N282" t="inlineStr">
+        <is>
+          <t>[sl 6855.85]</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2026.02.17 18:00:33</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>837432480</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E283" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F283" t="n">
+        <v>24439</v>
+      </c>
+      <c r="I283" t="inlineStr">
+        <is>
+          <t>2026.02.17 21:40:38</t>
+        </is>
+      </c>
+      <c r="J283" t="n">
+        <v>24781.01</v>
+      </c>
+      <c r="K283" t="n">
+        <v>0</v>
+      </c>
+      <c r="L283" t="n">
+        <v>0</v>
+      </c>
+      <c r="M283" t="n">
+        <v>-855.03</v>
+      </c>
+      <c r="N283" t="inlineStr">
+        <is>
+          <t>[sl 24781.01]</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2026.02.18 10:47:05</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>841215152</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E284" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F284" t="n">
+        <v>68124.91</v>
+      </c>
+      <c r="I284" t="inlineStr">
+        <is>
+          <t>2026.02.18 11:16:44</t>
+        </is>
+      </c>
+      <c r="J284" t="n">
+        <v>68382.13</v>
+      </c>
+      <c r="K284" t="n">
+        <v>0</v>
+      </c>
+      <c r="L284" t="n">
+        <v>0</v>
+      </c>
+      <c r="M284" t="n">
+        <v>128.61</v>
+      </c>
+      <c r="N284" t="inlineStr">
+        <is>
+          <t>[tp 68382.13]</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2026.02.18 15:06:23</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>842152650</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E285" t="n">
+        <v>10</v>
+      </c>
+      <c r="F285" t="n">
+        <v>24892.72</v>
+      </c>
+      <c r="I285" t="inlineStr">
+        <is>
+          <t>2026.02.18 15:34:04</t>
+        </is>
+      </c>
+      <c r="J285" t="n">
+        <v>24809.84</v>
+      </c>
+      <c r="K285" t="n">
+        <v>0</v>
+      </c>
+      <c r="L285" t="n">
+        <v>0</v>
+      </c>
+      <c r="M285" t="n">
+        <v>-828.8</v>
+      </c>
+      <c r="N285" t="inlineStr">
+        <is>
+          <t>[sl 24809.84]</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2026.02.18 15:59:36</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>842451778</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E286" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F286" t="n">
+        <v>4945.22</v>
+      </c>
+      <c r="I286" t="inlineStr">
+        <is>
+          <t>2026.02.18 16:15:34</t>
+        </is>
+      </c>
+      <c r="J286" t="n">
+        <v>4958.76</v>
+      </c>
+      <c r="K286" t="n">
+        <v>0</v>
+      </c>
+      <c r="L286" t="n">
+        <v>0</v>
+      </c>
+      <c r="M286" t="n">
+        <v>677</v>
+      </c>
+      <c r="N286" t="inlineStr">
+        <is>
+          <t>[tp 4958.76]</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2026.02.18 15:56:06</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>842420522</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>USDJPY</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E287" t="n">
+        <v>1</v>
+      </c>
+      <c r="F287" t="n">
+        <v>153.636</v>
+      </c>
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>2026.02.18 16:29:59</t>
+        </is>
+      </c>
+      <c r="J287" t="n">
+        <v>153.821</v>
+      </c>
+      <c r="K287" t="n">
+        <v>0</v>
+      </c>
+      <c r="L287" t="n">
+        <v>0</v>
+      </c>
+      <c r="M287" t="n">
+        <v>-120.27</v>
+      </c>
+      <c r="N287" t="inlineStr">
+        <is>
+          <t>[sl 153.821]</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2026.02.18 15:23:15</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>842259246</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E288" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F288" t="n">
+        <v>0.70761</v>
+      </c>
+      <c r="I288" t="inlineStr">
+        <is>
+          <t>2026.02.18 16:43:15</t>
+        </is>
+      </c>
+      <c r="J288" t="n">
+        <v>0.70638</v>
+      </c>
+      <c r="K288" t="n">
+        <v>0</v>
+      </c>
+      <c r="L288" t="n">
+        <v>0</v>
+      </c>
+      <c r="M288" t="n">
+        <v>-147.6</v>
+      </c>
+      <c r="N288" t="inlineStr">
+        <is>
+          <t>[sl 0.70638]</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2026.02.18 15:38:50</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>842339678</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E289" t="n">
+        <v>5</v>
+      </c>
+      <c r="F289" t="n">
+        <v>6867.95</v>
+      </c>
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>2026.02.18 18:04:15</t>
+        </is>
+      </c>
+      <c r="J289" t="n">
+        <v>6895.09</v>
+      </c>
+      <c r="K289" t="n">
+        <v>0</v>
+      </c>
+      <c r="L289" t="n">
+        <v>0</v>
+      </c>
+      <c r="M289" t="n">
+        <v>-135.7</v>
+      </c>
+      <c r="N289" t="inlineStr">
+        <is>
+          <t>[sl 6895.09]</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2026.02.19 11:27:43</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>846801653</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E290" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F290" t="n">
+        <v>66890.21000000001</v>
+      </c>
+      <c r="I290" t="inlineStr">
+        <is>
+          <t>2026.02.19 11:31:06</t>
+        </is>
+      </c>
+      <c r="J290" t="n">
+        <v>66889.71000000001</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0</v>
+      </c>
+      <c r="L290" t="n">
+        <v>0</v>
+      </c>
+      <c r="M290" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N290" t="inlineStr">
+        <is>
+          <t>[tp 66889.71]</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2026.02.19 11:49:03</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>846886478</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E291" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="F291" t="n">
+        <v>0.70746</v>
+      </c>
+      <c r="I291" t="inlineStr">
+        <is>
+          <t>2026.02.19 12:48:24</t>
+        </is>
+      </c>
+      <c r="J291" t="n">
+        <v>0.70573</v>
+      </c>
+      <c r="K291" t="n">
+        <v>0</v>
+      </c>
+      <c r="L291" t="n">
+        <v>0</v>
+      </c>
+      <c r="M291" t="n">
+        <v>-152.24</v>
+      </c>
+      <c r="N291" t="inlineStr">
+        <is>
+          <t>[sl 0.70573]</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2026.02.19 11:04:08</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>846715280</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E292" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="F292" t="n">
+        <v>5008.63</v>
+      </c>
+      <c r="I292" t="inlineStr">
+        <is>
+          <t>2026.02.19 13:09:19</t>
+        </is>
+      </c>
+      <c r="J292" t="n">
+        <v>4986.05</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0</v>
+      </c>
+      <c r="L292" t="n">
+        <v>0</v>
+      </c>
+      <c r="M292" t="n">
+        <v>-654.8200000000001</v>
+      </c>
+      <c r="N292" t="inlineStr">
+        <is>
+          <t>[sl 4986.05]</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2026.02.19 14:41:03</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>847627993</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E293" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F293" t="n">
+        <v>66720.45</v>
+      </c>
+      <c r="I293" t="inlineStr">
+        <is>
+          <t>2026.02.19 14:50:33</t>
+        </is>
+      </c>
+      <c r="J293" t="n">
+        <v>66561.44</v>
+      </c>
+      <c r="K293" t="n">
+        <v>0</v>
+      </c>
+      <c r="L293" t="n">
+        <v>0</v>
+      </c>
+      <c r="M293" t="n">
+        <v>79.51000000000001</v>
+      </c>
+      <c r="N293" t="inlineStr">
+        <is>
+          <t>[tp 66561.44]</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2026.02.19 14:36:27</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>847612918</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E294" t="n">
+        <v>2</v>
+      </c>
+      <c r="F294" t="n">
+        <v>602.74</v>
+      </c>
+      <c r="I294" t="inlineStr">
+        <is>
+          <t>2026.02.19 16:39:58</t>
+        </is>
+      </c>
+      <c r="J294" t="n">
+        <v>602.24</v>
+      </c>
+      <c r="K294" t="n">
+        <v>0</v>
+      </c>
+      <c r="L294" t="n">
+        <v>0</v>
+      </c>
+      <c r="M294" t="n">
+        <v>10</v>
+      </c>
+      <c r="N294" t="inlineStr">
+        <is>
+          <t>[tp 602.24]</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2026.02.19 15:02:42</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>847717544</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>AUDUSD</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E295" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F295" t="n">
+        <v>0.70435</v>
+      </c>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>2026.02.19 18:47:05</t>
+        </is>
+      </c>
+      <c r="J295" t="n">
+        <v>0.70635</v>
+      </c>
+      <c r="K295" t="n">
+        <v>0</v>
+      </c>
+      <c r="L295" t="n">
+        <v>0</v>
+      </c>
+      <c r="M295" t="n">
+        <v>-154</v>
+      </c>
+      <c r="N295" t="inlineStr">
+        <is>
+          <t>[sl 0.70635]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
data: mise à jour données runtime 23 février 2026
- deals_history, equity_log, trades_log, proposals_log
- sentiment cache (9 symboles)
- performance tracker, news calendar
- journal trades (13-21 fév)
- daily_loss_state (kill switch)
- report Excel mis à jour

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/reports/ReportHistory-10960352.xlsx
+++ b/reports/ReportHistory-10960352.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N295"/>
+  <dimension ref="A1:N305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026.02.20 06:10</t>
+          <t>2026.02.22 22:00</t>
         </is>
       </c>
     </row>
@@ -14376,6 +14376,486 @@
       <c r="N295" t="inlineStr">
         <is>
           <t>[sl 0.70635]</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2026.02.20 09:13:50</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>857029424</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E296" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F296" t="n">
+        <v>67885.42</v>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>2026.02.20 12:02:32</t>
+        </is>
+      </c>
+      <c r="J296" t="n">
+        <v>67986.69</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0</v>
+      </c>
+      <c r="L296" t="n">
+        <v>0</v>
+      </c>
+      <c r="M296" t="n">
+        <v>50.64</v>
+      </c>
+      <c r="N296" t="inlineStr">
+        <is>
+          <t>[tp 67986.69]</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2026.02.20 11:03:46</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>858034226</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>XAUUSD</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E297" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="F297" t="n">
+        <v>5015.08</v>
+      </c>
+      <c r="I297" t="inlineStr">
+        <is>
+          <t>2026.02.20 12:08:21</t>
+        </is>
+      </c>
+      <c r="J297" t="n">
+        <v>5036.92</v>
+      </c>
+      <c r="K297" t="n">
+        <v>0</v>
+      </c>
+      <c r="L297" t="n">
+        <v>0</v>
+      </c>
+      <c r="M297" t="n">
+        <v>567.84</v>
+      </c>
+      <c r="N297" t="inlineStr">
+        <is>
+          <t>closePosition</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2026.02.20 12:12:27</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>858453115</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E298" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F298" t="n">
+        <v>68139.89</v>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>2026.02.20 14:37:17</t>
+        </is>
+      </c>
+      <c r="J298" t="n">
+        <v>67700.03999999999</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0</v>
+      </c>
+      <c r="L298" t="n">
+        <v>0</v>
+      </c>
+      <c r="M298" t="n">
+        <v>-219.93</v>
+      </c>
+      <c r="N298" t="inlineStr">
+        <is>
+          <t>[sl 67700.04]</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2026.02.20 15:01:41</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>859203714</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>SP500</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E299" t="n">
+        <v>5</v>
+      </c>
+      <c r="F299" t="n">
+        <v>6854.85</v>
+      </c>
+      <c r="I299" t="inlineStr">
+        <is>
+          <t>2026.02.20 15:34:59</t>
+        </is>
+      </c>
+      <c r="J299" t="n">
+        <v>6852.96</v>
+      </c>
+      <c r="K299" t="n">
+        <v>0</v>
+      </c>
+      <c r="L299" t="n">
+        <v>0</v>
+      </c>
+      <c r="M299" t="n">
+        <v>9.449999999999999</v>
+      </c>
+      <c r="N299" t="inlineStr">
+        <is>
+          <t>closePosition</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2026.02.20 15:02:01</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>859205782</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>NAS100</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E300" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="F300" t="n">
+        <v>24756.27</v>
+      </c>
+      <c r="I300" t="inlineStr">
+        <is>
+          <t>2026.02.20 15:35:01</t>
+        </is>
+      </c>
+      <c r="J300" t="n">
+        <v>24752.07</v>
+      </c>
+      <c r="K300" t="n">
+        <v>0</v>
+      </c>
+      <c r="L300" t="n">
+        <v>0</v>
+      </c>
+      <c r="M300" t="n">
+        <v>41.58</v>
+      </c>
+      <c r="N300" t="inlineStr">
+        <is>
+          <t>closePosition</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2026.02.20 15:12:31</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>859258095</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>USDJPY</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E301" t="n">
+        <v>1</v>
+      </c>
+      <c r="F301" t="n">
+        <v>155.28</v>
+      </c>
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>2026.02.20 15:35:03</t>
+        </is>
+      </c>
+      <c r="J301" t="n">
+        <v>155.278</v>
+      </c>
+      <c r="K301" t="n">
+        <v>0</v>
+      </c>
+      <c r="L301" t="n">
+        <v>0</v>
+      </c>
+      <c r="M301" t="n">
+        <v>-1.29</v>
+      </c>
+      <c r="N301" t="inlineStr">
+        <is>
+          <t>closePosition</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2026.02.21 12:21:54</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>862813462</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E302" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F302" t="n">
+        <v>68250.86</v>
+      </c>
+      <c r="I302" t="inlineStr">
+        <is>
+          <t>2026.02.21 12:22:10</t>
+        </is>
+      </c>
+      <c r="J302" t="n">
+        <v>68251.36</v>
+      </c>
+      <c r="K302" t="n">
+        <v>0</v>
+      </c>
+      <c r="L302" t="n">
+        <v>0</v>
+      </c>
+      <c r="M302" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N302" t="inlineStr">
+        <is>
+          <t>[tp 68251.36]</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2026.02.21 12:32:00</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>862818851</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>BTCUSD</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E303" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F303" t="n">
+        <v>68238.96000000001</v>
+      </c>
+      <c r="I303" t="inlineStr">
+        <is>
+          <t>2026.02.21 12:40:05</t>
+        </is>
+      </c>
+      <c r="J303" t="n">
+        <v>68239.46000000001</v>
+      </c>
+      <c r="K303" t="n">
+        <v>0</v>
+      </c>
+      <c r="L303" t="n">
+        <v>0</v>
+      </c>
+      <c r="M303" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N303" t="inlineStr">
+        <is>
+          <t>[tp 68239.46]</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2026.02.21 16:36:07</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>862936210</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>SOLUSD</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E304" t="n">
+        <v>5</v>
+      </c>
+      <c r="F304" t="n">
+        <v>85.63</v>
+      </c>
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>2026.02.21 17:21:50</t>
+        </is>
+      </c>
+      <c r="J304" t="n">
+        <v>86.19</v>
+      </c>
+      <c r="K304" t="n">
+        <v>0</v>
+      </c>
+      <c r="L304" t="n">
+        <v>0</v>
+      </c>
+      <c r="M304" t="n">
+        <v>28</v>
+      </c>
+      <c r="N304" t="inlineStr">
+        <is>
+          <t>[tp 86.19]</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2026.02.21 14:31:06</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>862866373</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>BNBUSD</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E305" t="n">
+        <v>1</v>
+      </c>
+      <c r="F305" t="n">
+        <v>631.6799999999999</v>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>2026.02.21 19:06:15</t>
+        </is>
+      </c>
+      <c r="J305" t="n">
+        <v>623.33</v>
+      </c>
+      <c r="K305" t="n">
+        <v>0</v>
+      </c>
+      <c r="L305" t="n">
+        <v>0</v>
+      </c>
+      <c r="M305" t="n">
+        <v>-83.5</v>
+      </c>
+      <c r="N305" t="inlineStr">
+        <is>
+          <t>[sl 623.33]</t>
         </is>
       </c>
     </row>

</xml_diff>